<commit_message>
added to AZN, Hedge Funds, Patents
</commit_message>
<xml_diff>
--- a/BGNE.xlsx
+++ b/BGNE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\CODE\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4701D43-DA24-4835-B9D7-2B5C07E6E108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66958D0-EFB3-4FF0-A360-A5214D237B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7965" yWindow="6750" windowWidth="20310" windowHeight="9705" xr2:uid="{ECF363C9-B515-44DE-94FD-36ED756098F0}"/>
+    <workbookView xWindow="15075" yWindow="315" windowWidth="33330" windowHeight="20340" xr2:uid="{ECF363C9-B515-44DE-94FD-36ED756098F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -357,14 +357,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -372,7 +371,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -690,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2391AD9C-ECF7-494A-A17A-9227C0123BFA}">
   <dimension ref="B2:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
@@ -726,140 +724,130 @@
         <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>188</v>
+        <v>219.94</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6" t="s">
+      <c r="G3" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="6"/>
       <c r="K3" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="13">
-        <v>102.46286600000001</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>21</v>
+      <c r="L3" s="11">
+        <f>1349.64018/13</f>
+        <v>103.8184753846154</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
-      <c r="C4" s="6" t="s">
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="6"/>
       <c r="K4" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="11">
         <f>L2*L3</f>
-        <v>19263.018808000001</v>
-      </c>
-      <c r="M4" s="11"/>
+        <v>22833.83547609231</v>
+      </c>
+      <c r="M4" s="10"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6" t="s">
+      <c r="G5" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="6"/>
       <c r="K5" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="13">
-        <v>6252.2330000000002</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>21</v>
+      <c r="L5" s="11">
+        <f>4197.132+871.998</f>
+        <v>5069.1299999999992</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6" t="s">
+      <c r="G6" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="6"/>
       <c r="K6" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="13">
-        <v>608.99199999999996</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>21</v>
+      <c r="L6" s="11">
+        <f>441.275+208</f>
+        <v>649.27499999999998</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
+      <c r="H7" s="6"/>
       <c r="K7" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="11">
         <f>L4-L5+L6</f>
-        <v>13619.777808000001</v>
+        <v>18413.980476092314</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9" t="s">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="10"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
@@ -877,18 +865,16 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" s="5"/>
-      <c r="C10" s="6" t="s">
+      <c r="C10" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6" t="s">
+      <c r="E10" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="12" t="s">
+      <c r="G10" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="6"/>
       <c r="K10" t="s">
         <v>7</v>
       </c>
@@ -897,25 +883,17 @@
       <c r="B11" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6" t="s">
+      <c r="E11" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="7"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
-      <c r="C12" s="6" t="s">
+      <c r="C12" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7"/>
+      <c r="H12" s="6"/>
       <c r="K12" t="s">
         <v>8</v>
       </c>
@@ -924,92 +902,69 @@
       <c r="B13" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6" t="s">
+      <c r="E13" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="7"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="12" t="s">
+      <c r="E14" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="12" t="s">
+      <c r="E15" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="7"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="12" t="s">
+      <c r="E16" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="12" t="s">
+      <c r="E17" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="7"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="5"/>
-      <c r="C18" s="6" t="s">
+      <c r="C18" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="12" t="s">
+      <c r="E18" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="7"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9" t="s">
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="10"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1030,7 +985,7 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="14" width="9.140625" style="11"/>
+    <col min="3" max="14" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
@@ -1039,40 +994,40 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="N2" s="10" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1080,10 +1035,10 @@
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="10">
         <v>22.1</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="10">
         <v>104.3</v>
       </c>
     </row>
@@ -1091,10 +1046,10 @@
       <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <v>48.9</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="10">
         <v>87.6</v>
       </c>
     </row>

</xml_diff>